<commit_message>
on est de retour
</commit_message>
<xml_diff>
--- a/Data Sheet/Résultats Banc de Test.xlsx
+++ b/Data Sheet/Résultats Banc de Test.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/bc6bc325e90e7782/Documents/CC_Seby_2021/Data Sheet/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="120" documentId="13_ncr:1_{D78F1A65-18EC-49E9-A8C7-19EEECE77B48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{7F8A1E10-9F39-4279-8B8B-07EB535609EE}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="13_ncr:1_{D78F1A65-18EC-49E9-A8C7-19EEECE77B48}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{3AEFE9C1-DBFD-4E91-B864-69021651B513}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="12B" sheetId="1" r:id="rId1"/>
+    <sheet name="B" sheetId="1" r:id="rId1"/>
     <sheet name="HB" sheetId="2" r:id="rId2"/>
     <sheet name="Synthèse" sheetId="3" r:id="rId3"/>
   </sheets>
@@ -180,7 +180,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
-              <a:t>Caractéristique de déformation du crayon 12B</a:t>
+              <a:t>Caractéristique de déformation du crayon B</a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -262,8 +262,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="7.8914236040684566E-2"/>
-                  <c:y val="8.5102209845507926E-2"/>
+                  <c:x val="0.1139748158182813"/>
+                  <c:y val="6.8123228574674413E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -298,7 +298,7 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
-              <c:f>'12B'!$C$2:$C$10</c:f>
+              <c:f>B!$C$2:$C$10</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="9"/>
@@ -334,7 +334,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'12B'!$G$2:$G$10</c:f>
+              <c:f>B!$G$2:$G$10</c:f>
               <c:numCache>
                 <c:formatCode>0%</c:formatCode>
                 <c:ptCount val="9"/>
@@ -782,8 +782,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="5.4398775600620258E-2"/>
-                  <c:y val="0.12432481931066106"/>
+                  <c:x val="0.10213961106524089"/>
+                  <c:y val="5.3927095451996622E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1209,7 +1209,7 @@
             </a:pPr>
             <a:r>
               <a:rPr lang="fr-FR"/>
-              <a:t>Caractéristiques de déformation des crayons 2H et HB </a:t>
+              <a:t>Caractéristiques de déformation des crayons HB et B </a:t>
             </a:r>
           </a:p>
         </c:rich>
@@ -1294,8 +1294,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="8.7725554129522459E-2"/>
-                  <c:y val="-2.7980687838981722E-2"/>
+                  <c:x val="9.5067698035543019E-2"/>
+                  <c:y val="-4.3784256191901634E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1405,7 +1405,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>2H</c:v>
+            <c:v>B</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -1446,8 +1446,8 @@
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="8.6257125348318239E-2"/>
-                  <c:y val="4.1945002761589439E-2"/>
+                  <c:x val="9.0662411691930581E-2"/>
+                  <c:y val="4.3112727424731691E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:numFmt formatCode="General" sourceLinked="0"/>
@@ -1612,7 +1612,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="fr-FR"/>
-                  <a:t>Déformation</a:t>
+                  <a:t>Déformation (%)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1729,7 +1729,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="fr-FR"/>
-                  <a:t>R/R0</a:t>
+                  <a:t>R/R0 (%)</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -1812,6 +1812,37 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="fr-FR"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
@@ -3563,14 +3594,14 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>981075</xdr:colOff>
-      <xdr:row>10</xdr:row>
+      <xdr:colOff>1123950</xdr:colOff>
+      <xdr:row>9</xdr:row>
       <xdr:rowOff>23811</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>33</xdr:row>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -3603,16 +3634,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>619125</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>109536</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>76200</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>90486</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>14</xdr:col>
-      <xdr:colOff>180975</xdr:colOff>
-      <xdr:row>28</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:colOff>400050</xdr:colOff>
+      <xdr:row>29</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -3905,8 +3936,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G41"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H37" sqref="H37"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4207,7 +4238,7 @@
   <dimension ref="A1:G8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J13" sqref="J13"/>
+      <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4432,8 +4463,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2DE737AE-35C0-43A9-B3E7-6A33C307FB29}">
   <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q7" sqref="Q7"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I36" sqref="I36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>